<commit_message>
Moved FYP out of att_awe
</commit_message>
<xml_diff>
--- a/protocols/fmrichecklist.xlsx
+++ b/protocols/fmrichecklist.xlsx
@@ -168,7 +168,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -201,6 +201,11 @@
       <u/>
       <sz val="10"/>
       <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -880,10 +885,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:D89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="19.25" customHeight="1" x14ac:dyDescent="0"/>
@@ -1265,15 +1273,16 @@
     <row r="88" ht="12"/>
     <row r="89" ht="12"/>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup scale="93" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>

<commit_message>
Added some new  analysis and protocols
</commit_message>
<xml_diff>
--- a/protocols/fmrichecklist.xlsx
+++ b/protocols/fmrichecklist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="6380" yWindow="740" windowWidth="25500" windowHeight="20420" tabRatio="293"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>Session ID: s30020150304</t>
   </si>
@@ -84,10 +84,6 @@
     <t>Give subject earplugs</t>
   </si>
   <si>
-    <t>Enter subject info
-Retrieve experimental sequences (CNI software)</t>
-  </si>
-  <si>
     <t>Run experiment</t>
   </si>
   <si>
@@ -159,6 +155,15 @@
   </si>
   <si>
     <t>Adjust the large mirror at the back of the scanner to center screen horizontally</t>
+  </si>
+  <si>
+    <t>Test Button Box</t>
+  </si>
+  <si>
+    <t>Close Test Screen</t>
+  </si>
+  <si>
+    <t>Enter subject info + Get Sequences</t>
   </si>
 </sst>
 </file>
@@ -210,7 +215,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,8 +240,14 @@
         <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -297,21 +308,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="hair">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="hair">
         <color rgb="FF000000"/>
@@ -325,7 +321,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -345,8 +341,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -447,15 +453,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -468,8 +471,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -479,6 +486,11 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -488,6 +500,11 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -888,10 +905,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:D89"/>
+  <dimension ref="B1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="19.25" customHeight="1" x14ac:dyDescent="0"/>
@@ -906,7 +923,7 @@
     <row r="1" spans="2:4" ht="19.25" customHeight="1">
       <c r="B1" s="3"/>
       <c r="C1" s="39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" s="4"/>
     </row>
@@ -970,8 +987,8 @@
       <c r="B10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="46" t="s">
-        <v>34</v>
+      <c r="C10" s="45" t="s">
+        <v>33</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>9</v>
@@ -1015,7 +1032,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>9</v>
@@ -1031,21 +1048,21 @@
     <row r="18" spans="2:4" ht="12.75" customHeight="1">
       <c r="B18" s="4"/>
       <c r="C18" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="2:4" ht="12.75" customHeight="1">
       <c r="B19" s="4"/>
       <c r="C19" s="26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="2:4" ht="24">
       <c r="B20" s="4"/>
       <c r="C20" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="4"/>
     </row>
@@ -1057,28 +1074,28 @@
     <row r="22" spans="2:4" ht="12">
       <c r="B22" s="4"/>
       <c r="C22" s="37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="23"/>
     </row>
     <row r="23" spans="2:4" ht="12">
       <c r="B23" s="4"/>
-      <c r="C23" s="43" t="s">
-        <v>23</v>
+      <c r="C23" s="42" t="s">
+        <v>22</v>
       </c>
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="2:4" ht="12">
       <c r="B24" s="25"/>
-      <c r="C24" s="44" t="s">
-        <v>24</v>
+      <c r="C24" s="43" t="s">
+        <v>23</v>
       </c>
       <c r="D24" s="25"/>
     </row>
     <row r="25" spans="2:4" ht="12">
       <c r="B25" s="25"/>
-      <c r="C25" s="45" t="s">
-        <v>26</v>
+      <c r="C25" s="44" t="s">
+        <v>25</v>
       </c>
       <c r="D25" s="25"/>
     </row>
@@ -1090,148 +1107,147 @@
     <row r="27" spans="2:4" ht="12.75" customHeight="1">
       <c r="B27" s="16"/>
       <c r="C27" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" s="16"/>
     </row>
     <row r="28" spans="2:4" ht="12">
       <c r="B28" s="4"/>
       <c r="C28" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="2:4" ht="12">
       <c r="B29" s="4"/>
       <c r="C29" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="2:4" ht="30" customHeight="1">
       <c r="B30" s="4"/>
       <c r="C30" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="2:4" ht="15" customHeight="1">
+      <c r="B31" s="4"/>
+      <c r="C31" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="2:4" ht="12">
-      <c r="B31" s="17"/>
-      <c r="C31" s="29"/>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="2:4" ht="12.75" customHeight="1">
-      <c r="B32" s="16" t="s">
+    <row r="32" spans="2:4" ht="15" customHeight="1">
+      <c r="B32" s="4"/>
+      <c r="C32" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="2:4" ht="12">
+      <c r="B33" s="17"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="2:4" ht="12.75" customHeight="1">
+      <c r="B34" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C34" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D34" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="2:4" s="22" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B33" s="31"/>
-      <c r="C33" s="32" t="s">
+    <row r="35" spans="2:4" s="22" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B35" s="31"/>
+      <c r="C35" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="31"/>
-    </row>
-    <row r="34" spans="2:4" s="22" customFormat="1" ht="12">
-      <c r="B34" s="33"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="31"/>
-    </row>
-    <row r="35" spans="2:4" ht="12.75" customHeight="1">
-      <c r="B35" s="16" t="s">
+      <c r="D35" s="31"/>
+    </row>
+    <row r="36" spans="2:4" s="22" customFormat="1" ht="12">
+      <c r="B36" s="33"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="31"/>
+    </row>
+    <row r="37" spans="2:4" ht="17" customHeight="1">
+      <c r="B37" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C37" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="12">
+      <c r="B38" s="17"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="2:4" ht="12" customHeight="1">
+      <c r="B39" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="C39" s="35"/>
+      <c r="D39" s="7"/>
+    </row>
+    <row r="40" spans="2:4" ht="12">
+      <c r="B40" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="36" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="12">
-      <c r="B36" s="17"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="2:4" ht="12">
-      <c r="B37" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="35"/>
-      <c r="D37" s="7"/>
-    </row>
-    <row r="38" spans="2:4" ht="12">
-      <c r="B38" s="30"/>
-      <c r="C38" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D38" s="36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="23" customHeight="1">
-      <c r="B39" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="12">
-      <c r="B40" s="36"/>
-      <c r="C40" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="D40" s="36"/>
-    </row>
-    <row r="41" spans="2:4" ht="26" customHeight="1">
-      <c r="B41" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="27"/>
-      <c r="D41" s="4"/>
-    </row>
+    <row r="41" spans="2:4" ht="23" customHeight="1"/>
     <row r="42" spans="2:4" ht="12">
       <c r="B42" s="36"/>
       <c r="C42" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="36"/>
+    </row>
+    <row r="43" spans="2:4" ht="26" customHeight="1">
+      <c r="C43" s="27"/>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="2:4" ht="12">
+      <c r="B44" s="36"/>
+      <c r="C44" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="36"/>
+    </row>
+    <row r="45" spans="2:4" ht="22" customHeight="1">
+      <c r="B45"/>
+    </row>
+    <row r="46" spans="2:4" ht="12">
+      <c r="B46" s="36"/>
+      <c r="C46" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="D42" s="36"/>
-    </row>
-    <row r="43" spans="2:4" ht="22" customHeight="1">
-      <c r="B43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" ht="12">
-      <c r="B44" s="40"/>
-      <c r="C44" s="41" t="s">
+      <c r="D46" s="41"/>
+    </row>
+    <row r="47" spans="2:4" ht="25" customHeight="1">
+      <c r="B47"/>
+    </row>
+    <row r="48" spans="2:4" ht="12">
+      <c r="B48" s="36"/>
+      <c r="C48" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="D44" s="42"/>
-    </row>
-    <row r="45" spans="2:4" ht="25" customHeight="1">
-      <c r="B45" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" ht="12">
-      <c r="B46" s="40"/>
-      <c r="C46" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="D46" s="42"/>
-    </row>
-    <row r="47" spans="2:4" ht="33" customHeight="1">
-      <c r="B47" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" ht="12"/>
-    <row r="49" ht="12"/>
+      <c r="D48" s="41"/>
+    </row>
+    <row r="49" ht="33" customHeight="1"/>
     <row r="50" ht="12"/>
     <row r="51" ht="12"/>
     <row r="52" ht="12"/>
@@ -1272,10 +1288,12 @@
     <row r="87" ht="12"/>
     <row r="88" ht="12"/>
     <row r="89" ht="12"/>
+    <row r="90" ht="12"/>
+    <row r="91" ht="12"/>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup scale="93" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup scale="88" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>